<commit_message>
Ontbrekende velden zib Patient toegevoegd
</commit_message>
<xml_diff>
--- a/maps/Patient.xlsx
+++ b/maps/Patient.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\mgraauw\eu-nl-compared\maps\xtehr2zibs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\mgraauw\eu-nl-compared\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA628490-060F-40AE-BD11-81BF7A9AFAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADD4747-7FC1-4C3B-8394-0F48E3223956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20610" yWindow="3045" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>EHDSPatient</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>xtehr</t>
+  </si>
+  <si>
+    <t>Patient.GenderIdentity</t>
+  </si>
+  <si>
+    <t>Patient.MultipleBirthSequence</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +562,16 @@
         <v>19</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>